<commit_message>
Proctor Provisioning code added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/ExamTaker_Creation_at_procter_side_Details.xlsx
+++ b/src/test/resources/ExcelFiles/ExamTaker_Creation_at_procter_side_Details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="15924" windowHeight="5448" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="6396" windowHeight="4032"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F24"/>
+  <oleSize ref="A1:I13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Email</t>
   </si>
@@ -49,18 +49,6 @@
     <t>JUL</t>
   </si>
   <si>
-    <t>DEC</t>
-  </si>
-  <si>
-    <t>Location22</t>
-  </si>
-  <si>
-    <t>jan8examtaker@yopmail.com</t>
-  </si>
-  <si>
-    <t>Jan11</t>
-  </si>
-  <si>
     <t>BBSR</t>
   </si>
   <si>
@@ -68,6 +56,9 @@
   </si>
   <si>
     <t>222211</t>
+  </si>
+  <si>
+    <t>Chicago</t>
   </si>
 </sst>
 </file>
@@ -92,7 +83,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF1E88E5"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -433,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,28 +463,28 @@
     </row>
     <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4599</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>8897</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>2023</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>28</v>
+      <c r="F2" s="5">
+        <v>2008</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -511,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,10 +541,10 @@
     </row>
     <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -562,7 +553,7 @@
         <v>4599</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F2" s="5">
         <v>2008</v>

</xml_diff>